<commit_message>
modified LOD, LOQ, and debugged
</commit_message>
<xml_diff>
--- a/lib/APGCMS/APGCMS/lib/lib_serum_CalibrationCurve_20160322.xlsx
+++ b/lib/APGCMS/APGCMS/lib/lib_serum_CalibrationCurve_20160322.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="26060" yWindow="3280" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="27880" yWindow="2900" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="CalibrationCurve_Serum" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="100">
   <si>
     <t>rsq</t>
   </si>
@@ -317,6 +317,9 @@
   </si>
   <si>
     <t>RI</t>
+  </si>
+  <si>
+    <t>LOQ</t>
   </si>
 </sst>
 </file>
@@ -324,7 +327,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -388,8 +391,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="137">
+  <cellStyleXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -531,11 +536,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="137">
+  <cellStyles count="139">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -604,6 +609,7 @@
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -672,6 +678,7 @@
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1001,20 +1008,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -1025,7 +1033,7 @@
         <v>89</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E1" t="s">
         <v>90</v>
@@ -1042,8 +1050,11 @@
       <c r="I1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1053,8 +1064,8 @@
       <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="D2">
-        <v>1092.2</v>
+      <c r="D2" t="s">
+        <v>47</v>
       </c>
       <c r="E2" s="3">
         <v>0.105653836040106</v>
@@ -1071,8 +1082,11 @@
       <c r="I2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2">
+        <v>1092.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1082,8 +1096,8 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3">
-        <v>1103.4000000000001</v>
+      <c r="D3" t="s">
+        <v>47</v>
       </c>
       <c r="E3" s="3">
         <v>1.3204834990939499E-2</v>
@@ -1100,8 +1114,11 @@
       <c r="I3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3">
+        <v>1103.4000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1111,8 +1128,8 @@
       <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="D4">
-        <v>1111.5</v>
+      <c r="D4" t="s">
+        <v>47</v>
       </c>
       <c r="E4" s="3">
         <v>-2.8432894457239101E-2</v>
@@ -1129,8 +1146,11 @@
       <c r="I4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4">
+        <v>1111.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1140,8 +1160,8 @@
       <c r="C5" t="s">
         <v>51</v>
       </c>
-      <c r="D5">
-        <v>1131</v>
+      <c r="D5" t="s">
+        <v>47</v>
       </c>
       <c r="E5" s="3">
         <v>7.0115309111152893E-2</v>
@@ -1158,8 +1178,11 @@
       <c r="I5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1169,8 +1192,8 @@
       <c r="C6" t="s">
         <v>92</v>
       </c>
-      <c r="D6">
-        <v>1147.3</v>
+      <c r="D6" t="s">
+        <v>47</v>
       </c>
       <c r="E6" s="3">
         <v>0.116117414095851</v>
@@ -1187,8 +1210,11 @@
       <c r="I6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6">
+        <v>1147.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1198,8 +1224,8 @@
       <c r="C7" t="s">
         <v>35</v>
       </c>
-      <c r="D7">
-        <v>1167.5</v>
+      <c r="D7" t="s">
+        <v>47</v>
       </c>
       <c r="E7" s="3">
         <v>3.4287372093150199E-4</v>
@@ -1216,8 +1242,11 @@
       <c r="I7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7">
+        <v>1167.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1227,8 +1256,8 @@
       <c r="C8" t="s">
         <v>33</v>
       </c>
-      <c r="D8">
-        <v>1175.5999999999999</v>
+      <c r="D8" t="s">
+        <v>47</v>
       </c>
       <c r="E8" s="3">
         <v>-7.4621710506315206E-2</v>
@@ -1245,8 +1274,11 @@
       <c r="I8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8">
+        <v>1175.5999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1256,8 +1288,8 @@
       <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="D9">
-        <v>1188</v>
+      <c r="D9" t="s">
+        <v>47</v>
       </c>
       <c r="E9" s="3">
         <v>-5.58073121005844E-2</v>
@@ -1274,8 +1306,11 @@
       <c r="I9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1285,8 +1320,8 @@
       <c r="C10" t="s">
         <v>54</v>
       </c>
-      <c r="D10">
-        <v>1192.0999999999999</v>
+      <c r="D10" t="s">
+        <v>47</v>
       </c>
       <c r="E10" s="3">
         <v>-4.1329129816391898E-2</v>
@@ -1303,8 +1338,11 @@
       <c r="I10" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10">
+        <v>1192.0999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1314,8 +1352,8 @@
       <c r="C11" t="s">
         <v>38</v>
       </c>
-      <c r="D11">
-        <v>1260.0999999999999</v>
+      <c r="D11" t="s">
+        <v>47</v>
       </c>
       <c r="E11" s="3">
         <v>-3.5821716572109599E-2</v>
@@ -1332,8 +1370,11 @@
       <c r="I11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11">
+        <v>1260.0999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1343,8 +1384,8 @@
       <c r="C12" t="s">
         <v>70</v>
       </c>
-      <c r="D12">
-        <v>1292.8</v>
+      <c r="D12" t="s">
+        <v>47</v>
       </c>
       <c r="E12" s="3">
         <v>2.1090642121927398E-2</v>
@@ -1361,8 +1402,11 @@
       <c r="I12" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12">
+        <v>1292.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1372,8 +1416,8 @@
       <c r="C13" t="s">
         <v>73</v>
       </c>
-      <c r="D13">
-        <v>1327.8</v>
+      <c r="D13" t="s">
+        <v>47</v>
       </c>
       <c r="E13" s="3">
         <v>-1.5549571505129899E-3</v>
@@ -1390,8 +1434,11 @@
       <c r="I13" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13">
+        <v>1327.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1401,8 +1448,8 @@
       <c r="C14" t="s">
         <v>40</v>
       </c>
-      <c r="D14">
-        <v>1381.2</v>
+      <c r="D14" t="s">
+        <v>47</v>
       </c>
       <c r="E14" s="3">
         <v>-9.0612063137322493E-2</v>
@@ -1419,8 +1466,11 @@
       <c r="I14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14">
+        <v>1381.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1430,8 +1480,8 @@
       <c r="C15" t="s">
         <v>56</v>
       </c>
-      <c r="D15">
-        <v>1406.6</v>
+      <c r="D15" t="s">
+        <v>47</v>
       </c>
       <c r="E15" s="3">
         <v>-1.89615430770067E-2</v>
@@ -1448,8 +1498,11 @@
       <c r="I15" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15">
+        <v>1406.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1459,8 +1512,8 @@
       <c r="C16" t="s">
         <v>9</v>
       </c>
-      <c r="D16">
-        <v>1434.9</v>
+      <c r="D16" t="s">
+        <v>47</v>
       </c>
       <c r="E16" s="3">
         <v>6.3767717991318806E-2</v>
@@ -1477,8 +1530,11 @@
       <c r="I16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16">
+        <v>1434.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1488,8 +1544,8 @@
       <c r="C17" t="s">
         <v>15</v>
       </c>
-      <c r="D17">
-        <v>1507.7</v>
+      <c r="D17" t="s">
+        <v>47</v>
       </c>
       <c r="E17" s="3">
         <v>5.9307197914811503E-2</v>
@@ -1506,8 +1562,11 @@
       <c r="I17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17">
+        <v>1507.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1517,8 +1576,8 @@
       <c r="C18" t="s">
         <v>25</v>
       </c>
-      <c r="D18">
-        <v>1534.3</v>
+      <c r="D18" t="s">
+        <v>47</v>
       </c>
       <c r="E18" s="3">
         <v>-0.16671262253921601</v>
@@ -1535,8 +1594,11 @@
       <c r="I18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18">
+        <v>1534.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1546,8 +1608,8 @@
       <c r="C19" t="s">
         <v>58</v>
       </c>
-      <c r="D19">
-        <v>1569.5</v>
+      <c r="D19" t="s">
+        <v>47</v>
       </c>
       <c r="E19" s="3">
         <v>-0.224597763068139</v>
@@ -1564,8 +1626,11 @@
       <c r="I19" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19">
+        <v>1569.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1575,8 +1640,8 @@
       <c r="C20" t="s">
         <v>42</v>
       </c>
-      <c r="D20">
-        <v>1587.9</v>
+      <c r="D20" t="s">
+        <v>47</v>
       </c>
       <c r="E20" s="3">
         <v>2.6977678586215699E-2</v>
@@ -1593,8 +1658,11 @@
       <c r="I20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20">
+        <v>1587.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1604,8 +1672,8 @@
       <c r="C21" t="s">
         <v>83</v>
       </c>
-      <c r="D21">
-        <v>1593.2</v>
+      <c r="D21" t="s">
+        <v>47</v>
       </c>
       <c r="E21" s="3">
         <v>3.8945160178868801E-2</v>
@@ -1622,8 +1690,11 @@
       <c r="I21" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21">
+        <v>1593.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1633,8 +1704,8 @@
       <c r="C22" t="s">
         <v>44</v>
       </c>
-      <c r="D22">
-        <v>1629.9</v>
+      <c r="D22" t="s">
+        <v>47</v>
       </c>
       <c r="E22" s="3">
         <v>-0.127360017304158</v>
@@ -1651,8 +1722,11 @@
       <c r="I22" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22">
+        <v>1629.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1662,8 +1736,8 @@
       <c r="C23" t="s">
         <v>11</v>
       </c>
-      <c r="D23">
-        <v>1638.1</v>
+      <c r="D23" t="s">
+        <v>47</v>
       </c>
       <c r="E23" s="3">
         <v>-5.43188372096726E-3</v>
@@ -1680,8 +1754,11 @@
       <c r="I23" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23">
+        <v>1638.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1691,8 +1768,8 @@
       <c r="C24" t="s">
         <v>27</v>
       </c>
-      <c r="D24">
-        <v>1638.8</v>
+      <c r="D24" t="s">
+        <v>47</v>
       </c>
       <c r="E24" s="3">
         <v>-0.102993718197813</v>
@@ -1709,8 +1786,11 @@
       <c r="I24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24">
+        <v>1638.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1720,8 +1800,8 @@
       <c r="C25" t="s">
         <v>46</v>
       </c>
-      <c r="D25">
-        <v>1722.8</v>
+      <c r="D25" t="s">
+        <v>47</v>
       </c>
       <c r="E25" s="3">
         <v>-0.24549649232849399</v>
@@ -1738,8 +1818,11 @@
       <c r="I25" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25">
+        <v>1722.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1749,17 +1832,20 @@
       <c r="C26" t="s">
         <v>93</v>
       </c>
-      <c r="D26">
+      <c r="D26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J26">
         <v>1759.8</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1769,8 +1855,8 @@
       <c r="C27" t="s">
         <v>85</v>
       </c>
-      <c r="D27">
-        <v>1766.1</v>
+      <c r="D27" t="s">
+        <v>47</v>
       </c>
       <c r="E27" s="3">
         <v>-8.3520027219146406E-2</v>
@@ -1787,8 +1873,11 @@
       <c r="I27" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27">
+        <v>1766.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1798,8 +1887,8 @@
       <c r="C28" t="s">
         <v>17</v>
       </c>
-      <c r="D28">
-        <v>1848.8</v>
+      <c r="D28" t="s">
+        <v>47</v>
       </c>
       <c r="E28" s="3">
         <v>6.4647051219529406E-2</v>
@@ -1816,8 +1905,11 @@
       <c r="I28" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28">
+        <v>1848.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1827,8 +1919,8 @@
       <c r="C29" t="s">
         <v>60</v>
       </c>
-      <c r="D29">
-        <v>1899.6</v>
+      <c r="D29" t="s">
+        <v>47</v>
       </c>
       <c r="E29" s="3">
         <v>-0.54980592230234804</v>
@@ -1845,8 +1937,11 @@
       <c r="I29" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29">
+        <v>1899.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1856,8 +1951,8 @@
       <c r="C30" t="s">
         <v>77</v>
       </c>
-      <c r="D30">
-        <v>1911.9</v>
+      <c r="D30" t="s">
+        <v>47</v>
       </c>
       <c r="E30" s="3">
         <v>5.2472446721946897E-2</v>
@@ -1874,8 +1969,11 @@
       <c r="I30" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30">
+        <v>1911.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1885,8 +1983,8 @@
       <c r="C31" t="s">
         <v>79</v>
       </c>
-      <c r="D31">
-        <v>1926.6</v>
+      <c r="D31" t="s">
+        <v>47</v>
       </c>
       <c r="E31" s="3">
         <v>7.1578169689412705E-2</v>
@@ -1903,8 +2001,11 @@
       <c r="I31" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31">
+        <v>1926.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1914,8 +2015,8 @@
       <c r="C32" t="s">
         <v>13</v>
       </c>
-      <c r="D32">
-        <v>1931.8</v>
+      <c r="D32" t="s">
+        <v>47</v>
       </c>
       <c r="E32" s="3">
         <v>7.8650740789131299E-2</v>
@@ -1932,8 +2033,11 @@
       <c r="I32" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="J32">
+        <v>1931.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1943,8 +2047,8 @@
       <c r="C33" t="s">
         <v>29</v>
       </c>
-      <c r="D33">
-        <v>1938.8</v>
+      <c r="D33" t="s">
+        <v>47</v>
       </c>
       <c r="E33" s="3">
         <v>0.26854857528237702</v>
@@ -1961,8 +2065,11 @@
       <c r="I33" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="J33">
+        <v>1938.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1972,8 +2079,8 @@
       <c r="C34" t="s">
         <v>62</v>
       </c>
-      <c r="D34">
-        <v>2053.8000000000002</v>
+      <c r="D34" t="s">
+        <v>47</v>
       </c>
       <c r="E34" s="3">
         <v>-6.6157455305384597E-2</v>
@@ -1990,8 +2097,11 @@
       <c r="I34" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="J34">
+        <v>2053.8000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2001,8 +2111,8 @@
       <c r="C35" t="s">
         <v>75</v>
       </c>
-      <c r="D35" s="1">
-        <v>2124.3000000000002</v>
+      <c r="D35" t="s">
+        <v>47</v>
       </c>
       <c r="E35" s="3">
         <v>-7.5443548915921296E-2</v>
@@ -2019,8 +2129,11 @@
       <c r="I35" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="J35" s="1">
+        <v>2124.3000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2030,8 +2143,8 @@
       <c r="C36" t="s">
         <v>31</v>
       </c>
-      <c r="D36">
-        <v>2132.1999999999998</v>
+      <c r="D36" t="s">
+        <v>47</v>
       </c>
       <c r="E36" s="3">
         <v>0.30464316047904999</v>
@@ -2048,8 +2161,11 @@
       <c r="I36" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="1:10">
+      <c r="J36">
+        <v>2132.1999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2059,8 +2175,8 @@
       <c r="C37" t="s">
         <v>64</v>
       </c>
-      <c r="D37">
-        <v>2210</v>
+      <c r="D37" t="s">
+        <v>47</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>47</v>
@@ -2077,11 +2193,14 @@
       <c r="I37" t="s">
         <v>52</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J37">
+        <v>2210</v>
+      </c>
+      <c r="K37" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:11">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2091,23 +2210,26 @@
       <c r="C38" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D38">
+      <c r="D38" t="s">
+        <v>47</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G38" t="s">
+        <v>47</v>
+      </c>
+      <c r="H38" t="s">
+        <v>47</v>
+      </c>
+      <c r="J38">
         <v>2221</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G38" t="s">
-        <v>47</v>
-      </c>
-      <c r="H38" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2117,23 +2239,26 @@
       <c r="C39" t="s">
         <v>97</v>
       </c>
-      <c r="D39">
+      <c r="D39" t="s">
+        <v>47</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G39" t="s">
+        <v>47</v>
+      </c>
+      <c r="H39" t="s">
+        <v>47</v>
+      </c>
+      <c r="J39">
         <v>2248</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G39" t="s">
-        <v>47</v>
-      </c>
-      <c r="H39" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2143,8 +2268,8 @@
       <c r="C40" t="s">
         <v>81</v>
       </c>
-      <c r="D40" s="1">
-        <v>2765.2489999999998</v>
+      <c r="D40" t="s">
+        <v>47</v>
       </c>
       <c r="E40" s="3">
         <v>-0.167210136594722</v>
@@ -2161,8 +2286,11 @@
       <c r="I40" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="41" spans="1:10">
+      <c r="J40" s="1">
+        <v>2765.2489999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2172,8 +2300,8 @@
       <c r="C41" t="s">
         <v>49</v>
       </c>
-      <c r="D41">
-        <v>2817.5</v>
+      <c r="D41" t="s">
+        <v>47</v>
       </c>
       <c r="E41" s="3">
         <v>-0.32754358142394002</v>
@@ -2190,8 +2318,11 @@
       <c r="I41" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="42" spans="1:10">
+      <c r="J41">
+        <v>2817.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2201,8 +2332,8 @@
       <c r="C42" t="s">
         <v>67</v>
       </c>
-      <c r="D42">
-        <v>3161.9</v>
+      <c r="D42" t="s">
+        <v>47</v>
       </c>
       <c r="E42" s="3">
         <v>-3.9197187131406103E-2</v>
@@ -2219,11 +2350,11 @@
       <c r="I42" t="s">
         <v>68</v>
       </c>
+      <c r="J42">
+        <v>3161.9</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J42">
-    <sortCondition ref="D4"/>
-  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>